<commit_message>
Revert "WY wr update."
This reverts commit 39795115389d6a141ef847c11bcd235c82ed01bb.
</commit_message>
<xml_diff>
--- a/Wyoming/WaterAllocation/WY_POD_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Wyoming/WaterAllocation/WY_POD_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Wyoming\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BF6C0A-AF06-4B30-816C-E2B0349F9AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0065BE33-EA45-484F-AF91-B29B84F9FD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="3" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="523">
   <si>
     <t>Name</t>
   </si>
@@ -1658,15 +1658,6 @@
       </rPr>
       <t xml:space="preserve"> metadata, and anything with a Z in it also has a beneficial use = Wild and Scenic River</t>
     </r>
-  </si>
-  <si>
-    <t>WYwr_M1</t>
-  </si>
-  <si>
-    <t>WYwr_V1</t>
-  </si>
-  <si>
-    <t>Wywy_O1</t>
   </si>
 </sst>
 </file>
@@ -3291,8 +3282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3365,7 +3356,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3468,7 +3459,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>523</v>
+        <v>465</v>
       </c>
       <c r="F4" s="62" t="s">
         <v>38</v>
@@ -3760,7 +3751,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3857,7 +3848,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="104" t="s">
-        <v>524</v>
+        <v>442</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>38</v>
@@ -4172,8 +4163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BA2FE-2555-4166-A4DF-0203EE1C77D7}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4276,7 +4267,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>525</v>
+        <v>445</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>38</v>

</xml_diff>